<commit_message>
Atualização até o ID 358
</commit_message>
<xml_diff>
--- a/Web Scraping/NOVAS_Radar_PPP.xlsx
+++ b/Web Scraping/NOVAS_Radar_PPP.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liviabn\Pictures\Base_PPP\Web Scraping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A057F78B-1B8D-4971-94AE-0882A9500129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="256">
   <si>
     <t>Id</t>
   </si>
@@ -49,9 +55,6 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>Contratante e Contratada</t>
-  </si>
-  <si>
     <t>Setor</t>
   </si>
   <si>
@@ -334,66 +337,6 @@
     <t>R$180.000,00,</t>
   </si>
   <si>
-    <t>Alexandre Luz SPE Ltda. e a Prefeitura Municipal de Senador Alexandre Costa do Município de Senador Alexandre Costa para:</t>
-  </si>
-  <si>
-    <t>SPE Integra S.A. e a Secretaria Municipal de Governo - SGM e Secretaria Executiva de Desestatização e Parcerias - SEDPo - SEDP do Município de São Paulo para:</t>
-  </si>
-  <si>
-    <t>Jaraguá Luz Concessionária de Cidade Inteligente SPE Ltda. e a Prefeitura Municipal de Jaraguá do Município de Jaraguá para:</t>
-  </si>
-  <si>
-    <t>Concessionária de Iluminação Pública Conecta Campinas S.A. e a Secretaria Municipal de Gestão e Controle do Município de Campinas para:</t>
-  </si>
-  <si>
-    <t>Energia Limpa PPP SPE S.A. e a Secretaria Municipal de Administração Planejamento e Gestão - SEMAD do Município de Manaus para:</t>
-  </si>
-  <si>
-    <t>Renova Suzano Ambiental Ltda. e a Secretaria Municipal de Manutenção e Serviços Urbanos do Município de Suzano para:</t>
-  </si>
-  <si>
-    <t>Centro Norte Construção e Administração de Empreendimentos SPE Ltda. e a Procuradoria-Geral do Estado de Rondônia do Estado de Rondônia para:</t>
-  </si>
-  <si>
-    <t>Luz de Jaboatão Energia S.A. e a Empresa Municipal de Energia e Iluminação Pública - Emlume do Município de Jaboatão dos Guararapes para:</t>
-  </si>
-  <si>
-    <t>BAL Civap SPE Ltda. e a Consórcio Intermunicipal do Vale do Paranapanema - Civap do Consórcio Público de Assis para:</t>
-  </si>
-  <si>
-    <t>Iluminação Pública Dores do Indaiá e a Prefeitura Municipal de Dores do Indaiá do Município de Dores do Indaiá para:</t>
-  </si>
-  <si>
-    <t>Três M Ambiental Eireli e a Prefeitura Municipal de Correntina do Município de Correntina para:</t>
-  </si>
-  <si>
-    <t>Luz de Caruaru Energia S.A. e a Prefeitura Municipal de Caruaru:</t>
-  </si>
-  <si>
-    <t>Ilumina Patos - SPE S.A. e a Prefeitura Municipal de Patos de Minas do Município de Patos de Minas para:</t>
-  </si>
-  <si>
-    <t>Sonda Infovia Digital do Estado de MS Serviços de Transporte de Dados SPE S.A. e a Secretaria de Estado de Fazenda - Sefaz do Estado de para:</t>
-  </si>
-  <si>
-    <t>Basílios Luz SPE Ltda. e a Secretaria de Infraestrutura e Serviços Públicos do Município de São José dos Basílios para:</t>
-  </si>
-  <si>
-    <t>Portal do Araguaia Resíduos SPE Ltda. e a Prefeitura Municipal de Água Boa para:</t>
-  </si>
-  <si>
-    <t>Qluz Nova Serrana Concessionária de Cidade Inteligente SPE S.A. e a Prefeitura Municipal de Nova Serrana:</t>
-  </si>
-  <si>
-    <t>Três M Ambiental Eireli e a Secretaria Municipal de Infraestrutura do Município de São Félix do Coribe para:</t>
-  </si>
-  <si>
-    <t>Concessionária Smart CPGI SPE S.A. e a Consórcio Público para Gestão Integrada - CPGI do Consórcio Público de para:</t>
-  </si>
-  <si>
-    <t>Oeiras Luz SPE Ltda. e a Prefeitura Municipal de Oeiras do Município de Oeiras para:</t>
-  </si>
-  <si>
     <t>Iluminação Pública</t>
   </si>
   <si>
@@ -725,13 +668,133 @@
   </si>
   <si>
     <t>https://radarppp.com/resumo-de-contratos-de-ppps/iluminacao-publica-oeiras/</t>
+  </si>
+  <si>
+    <t>Contratante</t>
+  </si>
+  <si>
+    <t>Contratada</t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Senador Alexandre Costa do Município de Senador Alexandre Costa</t>
+  </si>
+  <si>
+    <t>Alexandre Luz SPE Ltda.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPE Integra S.A.  </t>
+  </si>
+  <si>
+    <t>Secretaria Municipal de Governo - SGM e Secretaria Executiva de Desestatização e Parcerias - SEDPo - SEDP do Município de São Paulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaraguá Luz Concessionária de Cidade Inteligente SPE Ltda. </t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Jaraguá do Município de Jaraguá</t>
+  </si>
+  <si>
+    <t>Concessionária de Iluminação Pública Conecta Campinas S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Secretaria Municipal de Gestão e Controle do Município de Campinas</t>
+  </si>
+  <si>
+    <t>Energia Limpa PPP SPE S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Secretaria Municipal de Administração Planejamento e Gestão - SEMAD do Município de Manaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renova Suzano Ambiental Ltda. </t>
+  </si>
+  <si>
+    <t>Secretaria Municipal de Manutenção e Serviços Urbanos do Município de Suzano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centro Norte Construção e Administração de Empreendimentos SPE Ltda. </t>
+  </si>
+  <si>
+    <t>Procuradoria-Geral do Estado de Rondônia do Estado de Rondônia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luz de Jaboatão Energia S.A. </t>
+  </si>
+  <si>
+    <t>Empresa Municipal de Energia e Iluminação Pública - Emlume do Município de Jaboatão dos Guararapes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAL Civap SPE Ltda. </t>
+  </si>
+  <si>
+    <t>Consórcio Intermunicipal do Vale do Paranapanema - Civap do Consórcio Público de Assis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iluminação Pública Dores do Indaiá </t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Dores do Indaiá do Município de Dores do Indaiá</t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Correntina do Município de Correntin</t>
+  </si>
+  <si>
+    <t>Luz de Caruaru Energia S.A.</t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Caruaru:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilumina Patos - SPE S.A. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefeitura Municipal de Patos de Minas do Município de Patos de Minas </t>
+  </si>
+  <si>
+    <t>Sonda Infovia Digital do Estado de MS Serviços de Transporte de Dados SPE S.A.</t>
+  </si>
+  <si>
+    <t>Secretaria de Estado de Fazenda - Sefaz do Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basílios Luz SPE Ltda. </t>
+  </si>
+  <si>
+    <t>Secretaria de Infraestrutura e Serviços Públicos do Município de São José dos Basílios</t>
+  </si>
+  <si>
+    <t>Portal do Araguaia Resíduos SPE Ltda.</t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Água Boa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oeiras Luz SPE Ltda. </t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Oeiras do Município de Oeiras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concessionária Smart CPGI SPE S.A. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Consórcio Público para Gestão Integrada - CPGI do Consórcio Público</t>
+  </si>
+  <si>
+    <t>Secretaria Municipal de Infraestrutura do Município de São Félix do Coribe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qluz Nova Serrana Concessionária de Cidade Inteligente SPE S.A. </t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Nova Serrana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -802,16 +865,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -853,7 +924,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -885,9 +956,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -919,6 +1008,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1094,14 +1201,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1136,1925 +1248,1988 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>339</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c r="E2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
         <v>77</v>
       </c>
-      <c r="J2" t="s">
-        <v>78</v>
-      </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L2" t="s">
-        <v>106</v>
+        <v>218</v>
       </c>
       <c r="M2" t="s">
-        <v>126</v>
+        <v>219</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R2" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="S2" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="T2" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="U2" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="V2" t="s">
+        <v>174</v>
+      </c>
+      <c r="W2" t="s">
+        <v>175</v>
+      </c>
+      <c r="X2" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="W2" t="s">
-        <v>199</v>
-      </c>
-      <c r="X2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>217</v>
-      </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>340</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" t="s">
         <v>77</v>
       </c>
-      <c r="J3" t="s">
-        <v>78</v>
-      </c>
       <c r="K3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L3" t="s">
-        <v>107</v>
+        <v>221</v>
       </c>
       <c r="M3" t="s">
-        <v>127</v>
+        <v>220</v>
       </c>
       <c r="N3" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="O3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R3" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="S3" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="T3" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="U3" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="V3" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W3" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="X3" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="Y3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>218</v>
+        <v>56</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" t="s">
         <v>77</v>
       </c>
-      <c r="J4" t="s">
-        <v>78</v>
-      </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L4" t="s">
-        <v>108</v>
+        <v>223</v>
       </c>
       <c r="M4" t="s">
-        <v>126</v>
+        <v>222</v>
       </c>
       <c r="N4" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q4" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="R4" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="S4" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
       <c r="T4" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="U4" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="V4" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W4" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="X4" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="Y4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>219</v>
+        <v>56</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>342</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L5" t="s">
-        <v>109</v>
+        <v>225</v>
       </c>
       <c r="M5" t="s">
-        <v>126</v>
+        <v>224</v>
       </c>
       <c r="N5" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q5" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="R5" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="S5" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="T5" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="U5" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="V5" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W5" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="X5" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="Y5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>220</v>
+        <v>56</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>343</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L6" t="s">
-        <v>110</v>
+        <v>227</v>
       </c>
       <c r="M6" t="s">
-        <v>128</v>
+        <v>226</v>
       </c>
       <c r="N6" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="O6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q6" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="R6" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="S6" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="T6" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="U6" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="V6" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W6" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="X6" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
       <c r="Y6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>221</v>
+        <v>56</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>344</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
-        <v>111</v>
+        <v>229</v>
       </c>
       <c r="M7" t="s">
-        <v>129</v>
+        <v>228</v>
       </c>
       <c r="N7" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="O7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q7" t="s">
-        <v>133</v>
+        <v>56</v>
       </c>
       <c r="R7" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="S7" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="T7" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="U7" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="V7" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W7" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="X7" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="Y7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>222</v>
+        <v>56</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>345</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L8" t="s">
-        <v>112</v>
+        <v>231</v>
       </c>
       <c r="M8" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="N8" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="O8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q8" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="R8" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="S8" t="s">
-        <v>167</v>
+        <v>128</v>
       </c>
       <c r="T8" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="U8" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="V8" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W8" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="X8" t="s">
-        <v>57</v>
+        <v>184</v>
       </c>
       <c r="Y8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>223</v>
+        <v>56</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>346</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L9" t="s">
-        <v>113</v>
+        <v>233</v>
       </c>
       <c r="M9" t="s">
-        <v>126</v>
+        <v>232</v>
       </c>
       <c r="N9" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q9" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="R9" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="S9" t="s">
-        <v>168</v>
+        <v>129</v>
       </c>
       <c r="T9" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="U9" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="V9" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W9" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
       <c r="X9" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="Y9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC9" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD9" s="2" t="s">
-        <v>224</v>
+        <v>56</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>347</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L10" t="s">
-        <v>114</v>
+        <v>235</v>
       </c>
       <c r="M10" t="s">
-        <v>129</v>
+        <v>234</v>
       </c>
       <c r="N10" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="O10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q10" t="s">
-        <v>136</v>
+        <v>56</v>
       </c>
       <c r="R10" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="S10" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="T10" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="U10" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="V10" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W10" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="X10" t="s">
-        <v>57</v>
+        <v>186</v>
       </c>
       <c r="Y10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>225</v>
+        <v>56</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>348</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" t="s">
         <v>77</v>
       </c>
-      <c r="J11" t="s">
-        <v>78</v>
-      </c>
       <c r="K11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L11" t="s">
-        <v>115</v>
+        <v>237</v>
       </c>
       <c r="M11" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="N11" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q11" t="s">
+        <v>56</v>
+      </c>
+      <c r="R11" t="s">
+        <v>110</v>
+      </c>
+      <c r="S11" t="s">
         <v>131</v>
       </c>
-      <c r="R11" t="s">
-        <v>152</v>
-      </c>
-      <c r="S11" t="s">
-        <v>57</v>
-      </c>
       <c r="T11" t="s">
-        <v>185</v>
+        <v>56</v>
       </c>
       <c r="U11" t="s">
-        <v>195</v>
+        <v>164</v>
       </c>
       <c r="V11" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W11" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="X11" t="s">
-        <v>57</v>
+        <v>187</v>
       </c>
       <c r="Y11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC11" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD11" s="2" t="s">
-        <v>226</v>
+        <v>56</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>349</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L12" t="s">
-        <v>116</v>
+        <v>238</v>
       </c>
       <c r="M12" t="s">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="N12" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="O12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S12" t="s">
-        <v>170</v>
+        <v>56</v>
       </c>
       <c r="T12" t="s">
-        <v>186</v>
+        <v>149</v>
       </c>
       <c r="U12" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="V12" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="W12" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="X12" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="Y12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD12" s="2" t="s">
-        <v>227</v>
+        <v>56</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>350</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L13" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="M13" t="s">
-        <v>126</v>
+        <v>239</v>
       </c>
       <c r="N13" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q13" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="R13" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="S13" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="T13" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="U13" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="V13" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W13" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
       <c r="X13" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="Y13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC13" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD13" s="2" t="s">
-        <v>228</v>
+        <v>56</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>351</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L14" t="s">
-        <v>118</v>
+        <v>242</v>
       </c>
       <c r="M14" t="s">
-        <v>126</v>
+        <v>241</v>
       </c>
       <c r="N14" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q14" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="R14" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="S14" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="T14" t="s">
-        <v>188</v>
+        <v>56</v>
       </c>
       <c r="U14" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="V14" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W14" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="X14" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="Y14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC14" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>229</v>
+        <v>56</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>352</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L15" t="s">
-        <v>119</v>
+        <v>244</v>
       </c>
       <c r="M15" t="s">
-        <v>128</v>
+        <v>243</v>
       </c>
       <c r="N15" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="O15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q15" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
       <c r="R15" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="S15" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="T15" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="U15" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="V15" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W15" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="X15" t="s">
-        <v>57</v>
+        <v>190</v>
       </c>
       <c r="Y15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>230</v>
+        <v>56</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>353</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L16" t="s">
-        <v>120</v>
+        <v>246</v>
       </c>
       <c r="M16" t="s">
-        <v>126</v>
+        <v>245</v>
       </c>
       <c r="N16" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q16" t="s">
-        <v>138</v>
+        <v>56</v>
       </c>
       <c r="R16" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="S16" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="T16" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="U16" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="V16" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W16" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
       <c r="X16" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
       <c r="Y16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD16" s="2" t="s">
-        <v>231</v>
+        <v>56</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>354</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L17" t="s">
-        <v>121</v>
+        <v>248</v>
       </c>
       <c r="M17" t="s">
-        <v>129</v>
+        <v>247</v>
       </c>
       <c r="N17" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="O17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q17" t="s">
-        <v>139</v>
+        <v>56</v>
       </c>
       <c r="R17" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="S17" t="s">
+        <v>136</v>
+      </c>
+      <c r="T17" t="s">
+        <v>153</v>
+      </c>
+      <c r="U17" t="s">
+        <v>170</v>
+      </c>
+      <c r="V17" t="s">
         <v>174</v>
       </c>
-      <c r="T17" t="s">
-        <v>191</v>
-      </c>
-      <c r="U17" t="s">
-        <v>195</v>
-      </c>
-      <c r="V17" t="s">
-        <v>197</v>
-      </c>
       <c r="W17" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="X17" t="s">
-        <v>57</v>
+        <v>192</v>
       </c>
       <c r="Y17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC17" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD17" s="2" t="s">
-        <v>232</v>
+        <v>56</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>355</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" t="s">
         <v>77</v>
       </c>
-      <c r="J18" t="s">
-        <v>78</v>
-      </c>
       <c r="K18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L18" t="s">
-        <v>122</v>
+        <v>255</v>
       </c>
       <c r="M18" t="s">
-        <v>126</v>
+        <v>254</v>
       </c>
       <c r="N18" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q18" t="s">
-        <v>140</v>
+        <v>56</v>
       </c>
       <c r="R18" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
       <c r="S18" t="s">
+        <v>137</v>
+      </c>
+      <c r="T18" t="s">
+        <v>154</v>
+      </c>
+      <c r="U18" t="s">
+        <v>142</v>
+      </c>
+      <c r="V18" t="s">
+        <v>174</v>
+      </c>
+      <c r="W18" t="s">
         <v>175</v>
       </c>
-      <c r="T18" t="s">
-        <v>163</v>
-      </c>
-      <c r="U18" t="s">
-        <v>195</v>
-      </c>
-      <c r="V18" t="s">
-        <v>196</v>
-      </c>
-      <c r="W18" t="s">
-        <v>214</v>
-      </c>
       <c r="X18" t="s">
-        <v>57</v>
+        <v>193</v>
       </c>
       <c r="Y18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC18" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD18" s="2" t="s">
-        <v>233</v>
+        <v>56</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>356</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L19" t="s">
-        <v>123</v>
+        <v>253</v>
       </c>
       <c r="M19" t="s">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="N19" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="O19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T19" t="s">
-        <v>192</v>
+        <v>56</v>
       </c>
       <c r="U19" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="V19" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="W19" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="X19" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="Y19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC19" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD19" s="2" t="s">
-        <v>234</v>
+        <v>56</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE19" s="2" t="s">
+        <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>357</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" t="s">
         <v>76</v>
       </c>
-      <c r="H20" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>77</v>
       </c>
-      <c r="J20" t="s">
-        <v>78</v>
-      </c>
       <c r="K20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L20" t="s">
-        <v>124</v>
+        <v>252</v>
       </c>
       <c r="M20" t="s">
-        <v>126</v>
+        <v>251</v>
       </c>
       <c r="N20" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="O20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q20" t="s">
-        <v>141</v>
+        <v>56</v>
       </c>
       <c r="R20" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="S20" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="T20" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="U20" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="V20" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="W20" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="X20" t="s">
-        <v>57</v>
+        <v>194</v>
       </c>
       <c r="Y20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC20" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD20" s="2" t="s">
-        <v>235</v>
+        <v>56</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE20" s="2" t="s">
+        <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>358</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K21" t="s">
+        <v>104</v>
+      </c>
+      <c r="L21" t="s">
+        <v>250</v>
+      </c>
+      <c r="M21" t="s">
+        <v>249</v>
+      </c>
+      <c r="N21" t="s">
         <v>105</v>
       </c>
-      <c r="L21" t="s">
-        <v>125</v>
-      </c>
-      <c r="M21" t="s">
-        <v>126</v>
-      </c>
-      <c r="N21" t="s">
-        <v>57</v>
-      </c>
       <c r="O21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q21" t="s">
-        <v>142</v>
+        <v>56</v>
       </c>
       <c r="R21" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="S21" t="s">
-        <v>57</v>
+        <v>139</v>
       </c>
       <c r="T21" t="s">
-        <v>194</v>
+        <v>56</v>
       </c>
       <c r="U21" t="s">
+        <v>173</v>
+      </c>
+      <c r="V21" t="s">
+        <v>174</v>
+      </c>
+      <c r="W21" t="s">
+        <v>175</v>
+      </c>
+      <c r="X21" t="s">
         <v>195</v>
       </c>
-      <c r="V21" t="s">
-        <v>196</v>
-      </c>
-      <c r="W21" t="s">
-        <v>216</v>
-      </c>
-      <c r="X21" t="s">
-        <v>57</v>
-      </c>
       <c r="Y21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC21" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD21" s="2" t="s">
-        <v>236</v>
+        <v>56</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE21" s="2" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AD2" r:id="rId1"/>
-    <hyperlink ref="AD3" r:id="rId2"/>
-    <hyperlink ref="AD4" r:id="rId3"/>
-    <hyperlink ref="AD5" r:id="rId4"/>
-    <hyperlink ref="AD6" r:id="rId5"/>
-    <hyperlink ref="AD7" r:id="rId6"/>
-    <hyperlink ref="AD8" r:id="rId7"/>
-    <hyperlink ref="AD9" r:id="rId8"/>
-    <hyperlink ref="AD10" r:id="rId9"/>
-    <hyperlink ref="AD11" r:id="rId10"/>
-    <hyperlink ref="AD12" r:id="rId11"/>
-    <hyperlink ref="AD13" r:id="rId12"/>
-    <hyperlink ref="AD14" r:id="rId13"/>
-    <hyperlink ref="AD15" r:id="rId14"/>
-    <hyperlink ref="AD16" r:id="rId15"/>
-    <hyperlink ref="AD17" r:id="rId16"/>
-    <hyperlink ref="AD18" r:id="rId17"/>
-    <hyperlink ref="AD19" r:id="rId18"/>
-    <hyperlink ref="AD20" r:id="rId19"/>
-    <hyperlink ref="AD21" r:id="rId20"/>
+    <hyperlink ref="AE2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="AE3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="AE4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="AE5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="AE6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="AE7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="AE8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="AE9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="AE10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="AE11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="AE12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="AE13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="AE14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="AE15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="AE16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="AE17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="AE18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="AE19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="AE20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="AE21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>